<commit_message>
add simulation 1~9 result
</commit_message>
<xml_diff>
--- a/Env_Result.xlsx
+++ b/Env_Result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejl1\OneDrive\바탕 화면\FCP_simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이의준\Desktop\FCP_simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC11E88D-5977-4801-81E3-22EF4B85FACC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8018AC9-1332-41D9-96EC-D048ECC7BEB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4248" yWindow="600" windowWidth="14076" windowHeight="10644" xr2:uid="{1AA4E562-DF57-4E5C-8888-2449FF221874}"/>
+    <workbookView xWindow="2010" yWindow="540" windowWidth="26790" windowHeight="10740" xr2:uid="{1AA4E562-DF57-4E5C-8888-2449FF221874}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>UST_pool</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,6 +85,10 @@
   </si>
   <si>
     <t>block_reg*10(1min = 10block)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>각 트레이드에 대한 유동성을 24시간에 나눠서 분배</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -92,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +138,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +157,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -157,15 +174,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -196,24 +216,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="나쁨" xfId="1" builtinId="27"/>
+    <cellStyle name="보통" xfId="2" builtinId="28"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,52 +553,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95963207-D576-49E7-8089-624CCCF666EB}">
-  <dimension ref="A2:Q24"/>
+  <dimension ref="A2:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.3984375" customWidth="1"/>
-    <col min="4" max="4" width="13.8984375" customWidth="1"/>
-    <col min="6" max="6" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.09765625" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.125" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="23.59765625" customWidth="1"/>
+    <col min="10" max="10" width="23.625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="13.19921875" customWidth="1"/>
-    <col min="13" max="13" width="11.796875" customWidth="1"/>
+    <col min="12" max="12" width="13.25" customWidth="1"/>
+    <col min="13" max="13" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="19.2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="19.2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -607,32 +634,32 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="15">
         <v>1</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="16">
         <v>20000000</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="16">
         <v>1.5E-3</v>
       </c>
-      <c r="F4" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G4" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="F4" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G4" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H4" s="16">
         <v>1000000</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="16">
         <v>3000</v>
       </c>
       <c r="J4" s="5"/>
@@ -644,30 +671,30 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A5" s="11"/>
-      <c r="B5" s="6">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="16">
         <v>20000000</v>
       </c>
-      <c r="E5" s="7">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F5" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G5" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H5" s="7">
+      <c r="E5" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F5" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G5" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H5" s="16">
         <v>1000000</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="16">
         <v>3000</v>
       </c>
       <c r="J5" s="5"/>
@@ -679,30 +706,30 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15">
         <v>3</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="16">
         <v>20000000</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="16">
         <v>1E-3</v>
       </c>
-      <c r="F6" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G6" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H6" s="7">
+      <c r="F6" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G6" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H6" s="16">
         <v>1000000</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="16">
         <v>3000</v>
       </c>
       <c r="J6" s="5"/>
@@ -714,32 +741,32 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="15">
         <v>4</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="16">
         <v>20000000</v>
       </c>
-      <c r="E7" s="7">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F7" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G7" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H7" s="7">
-        <v>750000</v>
-      </c>
-      <c r="I7" s="7">
+      <c r="E7" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F7" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G7" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H7" s="16">
+        <v>1250000</v>
+      </c>
+      <c r="I7" s="16">
         <v>2500</v>
       </c>
       <c r="J7" s="5"/>
@@ -751,30 +778,30 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="6">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15">
         <v>5</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="16">
         <v>20000000</v>
       </c>
-      <c r="E8" s="7">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F8" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G8" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H8" s="7">
-        <v>100000</v>
-      </c>
-      <c r="I8" s="7">
+      <c r="E8" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F8" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G8" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H8" s="16">
+        <v>1000000</v>
+      </c>
+      <c r="I8" s="16">
         <v>2000</v>
       </c>
       <c r="J8" s="5"/>
@@ -786,30 +813,30 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A9" s="11"/>
-      <c r="B9" s="6">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15">
         <v>6</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="16">
         <v>20000000</v>
       </c>
-      <c r="E9" s="7">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F9" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G9" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="E9" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G9" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H9" s="16">
         <v>750000</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="16">
         <v>1500</v>
       </c>
       <c r="J9" s="1"/>
@@ -821,30 +848,30 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A10" s="11"/>
-      <c r="B10" s="6">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15">
         <v>7</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="16">
         <v>20000000</v>
       </c>
-      <c r="E10" s="7">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F10" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G10" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H10" s="7">
+      <c r="E10" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F10" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G10" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H10" s="16">
         <v>625000</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="16">
         <v>1250</v>
       </c>
       <c r="J10" s="1"/>
@@ -856,30 +883,30 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A11" s="11"/>
-      <c r="B11" s="6">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15">
         <v>8</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="16">
         <v>20000000</v>
       </c>
-      <c r="E11" s="7">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F11" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G11" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H11" s="7">
+      <c r="E11" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F11" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G11" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H11" s="16">
         <v>500000</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="16">
         <v>1000</v>
       </c>
       <c r="J11" s="1"/>
@@ -891,30 +918,30 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="6">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15">
         <v>9</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="16">
         <v>10000000000</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="16">
         <v>20000000</v>
       </c>
-      <c r="E12" s="7">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="F12" s="7">
-        <v>2000000000</v>
-      </c>
-      <c r="G12" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H12" s="7">
+      <c r="E12" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F12" s="16">
+        <v>2000000000</v>
+      </c>
+      <c r="G12" s="16">
+        <v>100000</v>
+      </c>
+      <c r="H12" s="16">
         <v>250000</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="16">
         <v>500</v>
       </c>
       <c r="J12" s="1"/>
@@ -926,20 +953,20 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="6">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -949,18 +976,18 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
       <c r="B14" s="6">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -970,18 +997,18 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
       <c r="B15" s="6">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -991,8 +1018,8 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A16" s="12"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
       <c r="B16" s="6">
         <v>13</v>
       </c>
@@ -1026,8 +1053,8 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
       <c r="B17" s="6">
         <v>14</v>
       </c>
@@ -1061,8 +1088,8 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
       <c r="B18" s="6">
         <v>15</v>
       </c>
@@ -1096,7 +1123,7 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>16</v>
       </c>
@@ -1130,7 +1157,7 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <v>17</v>
       </c>
@@ -1164,7 +1191,7 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <v>18</v>
       </c>
@@ -1198,7 +1225,7 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <v>19</v>
       </c>
@@ -1232,7 +1259,7 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <v>20</v>
       </c>
@@ -1266,7 +1293,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <v>21</v>
       </c>
@@ -1292,14 +1319,19 @@
         <v>5000</v>
       </c>
     </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A7:A12"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A7:A12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>